<commit_message>
v0.1.0, add all calculation
</commit_message>
<xml_diff>
--- a/Перечень VRS-500-019-01.xlsx
+++ b/Перечень VRS-500-019-01.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,10 +421,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="35" customWidth="1" min="2" max="2"/>
-    <col width="7" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
+    <col width="40" customWidth="1" min="1" max="1"/>
+    <col width="40" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -644,6 +644,1254 @@
       <c r="D12" t="inlineStr">
         <is>
           <t>нерж 2,0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Блок вентилятора ВОСК 2.5 АИР56</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ВХ 500.05.00.001.01-019*2.5</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Направляющая ВОСК 62,72,92</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>оц 3,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ВХ 500.05.00.002.01-019*2.5</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Панель ВОСК 62,72,92 ВЕРОСА 500</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>оц 1,5+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ВХ 500.05.00.003.01-2,5</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Кронштейн обратный </t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>оц 3,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ИНББ 230.00.00.001А-01</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Опора</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>ОЦ 2,0 + RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ИНББ 230.00.00.002А-01</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Уголок</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>ОЦ 3,0 + RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>ИНББ 230.00.00.003А-04</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Швеллер</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>ОЦ 3,0 + RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ИНББ 230.00.00.003А-05</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Швеллер</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>ОЦ 3,0 + RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>ИНББ 230.00.00.00.004А-04</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Плита подмоторная</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>ОЦ 3,0 + RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>ИН 761.00.00.003А-10</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Компенсатор</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>4</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ОЦ 1,0 + RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Блок вентилятора ВОСК 2.5 АИР56</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ВХ 500.05.00.001.01-019*2.5</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Направляющая ВОСК 62,72,92</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>оц 3,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>ВХ 500.05.00.002.01-019*2.5</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Панель ВОСК 62,72,92 ВЕРОСА 500</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>оц 1,5+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ВХ 500.05.00.003.01-2,5</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Кронштейн обратный </t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>2</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>оц 3,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>ИНББ 230.00.00.001А-01</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Опора</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>ОЦ 2,0 + RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>ИНББ 230.00.00.002А-01</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Уголок</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>ОЦ 3,0 + RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>ИНББ 230.00.00.003А-04</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Швеллер</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>ОЦ 3,0 + RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>ИНББ 230.00.00.003А-05</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Швеллер</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>ОЦ 3,0 + RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>ИНББ 230.00.00.00.004А-04</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Плита подмоторная</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>ОЦ 3,0 + RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>ИН 761.00.00.003А-10</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Компенсатор</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>4</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>ОЦ 1,0 + RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Блок ВНВ 5012</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ВХ 500.02.00.001.01-019х361</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Щиток ВНВ 1</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>оц 1,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>ВХ 500.02.00.002.01-019х361</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Щиток ВНВ 2</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>оц 1,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>ВХ 500.02.00.003.02-019х647x167</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Нижняя направляющая внв</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>нерж 1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>ВХ 500.02.00.004.02-019х647x167</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Верхняя направляющая внв </t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>нерж 1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Блок ВОВ 5012</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>ВХ 500.02.00.001.01-019х361</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Щиток ВНВ 1</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>оц 1,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>ВХ 500.02.00.002.01-019х361</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Щиток ВНВ 2</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>оц 1,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>ВХ 500.01.00.005.02-019х647х186</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">верхняя направляющая то </t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>нерж  1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>ВХ 500.01.00.006.02-019х647</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">верхняя направляющая каплеотделителя </t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>нерж  1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>ВХ 500.01.00.007.02-019*647</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>нижняя направляющая каплеотделителя</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>нерж  1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>ВХ 500.01.00.008.02-019x647х186</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>нижняя направляющая теплообменника</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>нерж  1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>ВХ 500.01.20.001.02-019</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>стенка верхняя</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>нерж  1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>ВХ 500.01.20.002.02-019</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>стенка нижняя</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>нерж  1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>ВХ 500.01.20.003.02-019</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>стенка вертикальная</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>2</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>нерж  1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>ТЕКИ 07.540.01.00.000</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Защитный кожух сливного комплекта</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>оц 2,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Блок ЭКО</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>ВХ 500.03.11.001.01-019</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Карта</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>2</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>оц 1,5+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ВХ 00.500.03.11.002.01-019</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Подставка</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>оц 1,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>ВХ 500.03.11.002.01-019</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Подставка</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>оц 1,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>ВХ 00.500.03.11.003.02-019</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Направляющая</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>нерж 1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>ВХ 500.03.11.003.02-019</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Направляющая</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>1</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>нерж 1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>ВХ 00.500.03.11.004.02-019</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Упор</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>нерж 2,0</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>ВХ 500.03.11.004.02-019</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Упор</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>1</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>нерж 2,0</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>ВХ 500.03.11.007.02-№</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Рычаг малый</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>2</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>нерж 2,0</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>ВХ 500.03.11.006.02-№</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Рычаг</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>2</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>нерж 2,0</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Блок вертикального клапана</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>ВХ 500.07.00.001.02-019</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Пластина</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>1</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>нерж 1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>ВХ 500.07.00.001.02-01*019</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Пластина</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>нерж 1,5</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>ВХ 500.07.00.002.01-019</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Уголок</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>1</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>оц 1,5+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>ВХ 500.07.00.002.01-01*019</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Уголок</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>оц 1,5+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>ВХ 500.07.00.003.01-019</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Уголок задний</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>1</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>оц 1,5+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>ВХ 500.07.00.004.01-019</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Уголок передний</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>1</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>оц 1,5+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>ВХ 500.07.00.005.01-019</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Зажим</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>1</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>оц 1,5+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>ВХ 500.07.00.005.01-01*019</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Зажим</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>1</v>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>оц 1,5+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>ВХ 500.07.00.006.01</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Рычаг</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>2</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>оц 3,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Блок пластинчатого утилизатора</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>ВХ 500.11.00.001.01-019</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Уголок клапана</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>1</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>оц 1,5+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>ВХ 500.11.00.002.01-019</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Лист байпасса</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>2</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>оц 2,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>ВХ 500.11.00.003.02-147*645*019</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Стойка боковая</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>4</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>нерж 2,0</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>ВХ 500.11.00.004.02-159*645*019</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Стойка вертикальная</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>2</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>нерж 2,0</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>ВХ 500.11.00.005.02-155*645*019</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>Стойка вертикальная укороченная</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>1</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>нерж 2,0</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>ВХ 500.11.00.006.02-159*645*019</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Стойка вертикальная с перфорацией</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>1</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>нерж 2,0</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>ТЕКИ 07.540.01.00.000</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Защитный кожух сливного комплекта</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>2</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>оц 2,0+RAL</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Блок камеры промежуточной</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>ВХ 500.16.00.001.01-019*555*647</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Лист отбойный</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>1</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>оц 0,7+RAL</t>
         </is>
       </c>
     </row>

</xml_diff>